<commit_message>
4.- actualizando el documento de historias de usuarios v1.2 de la aplicación
</commit_message>
<xml_diff>
--- a/Documentos/PETAPP_HU_01.xlsx
+++ b/Documentos/PETAPP_HU_01.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elvis\Documents\Repositorios\Trabajo_Evolucion_Cliente\Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elvis\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="12420"/>
   </bookViews>
   <sheets>
-    <sheet name="Historias de usuario" sheetId="1" r:id="rId1"/>
+    <sheet name="Historias de usuario" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
   <si>
     <t>HU01</t>
   </si>
@@ -44,46 +44,85 @@
     <t>HU06</t>
   </si>
   <si>
-    <t>Como usuario debe permitir ingresar a la aplicación web con mi cuenta de usuario y mi contraseña que ya han sido registrados en la base de datos.</t>
-  </si>
-  <si>
-    <t>Como administrador debo eliminar cuentas de usuarios inactivos que no cuenta con una membresia de pago; con la finalizadad de mejorar los tiempos de busquedas entre los mascotas de los usuarios.</t>
-  </si>
-  <si>
-    <t>Como un usuario registrado debo poder realizar busquedas de canes según los filtros que establezca para la busqueda que pueden ser: raza, sexo, edad, peso, ubicación del dueño.</t>
-  </si>
-  <si>
-    <t>Como usuario debo poder saber el motivo por el cual no puedo acceder a mi cuenta de usuario debido a inactividad, mal comportamiento u otros; además, me permita proceder a una solución si hubiera oportunidad.</t>
-  </si>
-  <si>
-    <t>Como usuario debe permitir mostrar un panel de control con un menu donde pueda ver mi información personales, mis mascotas, configuraciones y buscar otras mascotas.</t>
-  </si>
-  <si>
-    <t>Como administrador debo poder bloquear usuarios que presenten un comportamiento indebido para evitar la mala experiencia de los usuarios en el sitio. Dentro de la web se considera mal comportamiento. Por ejemplo, escribir una publicación ofendiendo a la mascota o al dueño de la mascota. Proporcionar información falsa en alguna publicación realizada. Denunciar de forma errónea y/o sin responsabilidad a algún usuario sin que este allá cometido algún mal comportamiento.</t>
-  </si>
-  <si>
     <t>HU07</t>
   </si>
   <si>
-    <t>Como usuario debe permitir registrar un cuenta de usuario con un nombre de usuario, contraseña, nombre, apellido, genero, ubicación y correo electronico.</t>
-  </si>
-  <si>
     <t>HU08</t>
   </si>
   <si>
-    <t>Como usuario debe permitir ver información mas detalla de las mascotas que quiero escoger para el cruce como: ¿A quien le pertenece la mascota?, ¿Cómo me contacto con el dueño?, ¿Por qué distrito vive el dueño?, tambien un album de fotos de la mascota para saber en que condiciones se encuentra.</t>
-  </si>
-  <si>
     <t>HU09</t>
   </si>
   <si>
-    <t>Como usuario debe ver la reputación que pueda tener el dueño u opiniones de otros usuarios con respecto al trato de esta persona; así, si el estado de su mascota se encuentra sano, limpio y bien alimentado.</t>
-  </si>
-  <si>
     <t>Característica / Funcionalidad</t>
   </si>
   <si>
     <t>Identificador (ID) de la Historia</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Razón / Resultado</t>
+  </si>
+  <si>
+    <t>Como un usuario</t>
+  </si>
+  <si>
+    <t>Como un administrador</t>
+  </si>
+  <si>
+    <t>Necesito registrar un cuenta de usuario con un nombre de usuario, contraseña, nombre, apellido, genero, ubicación y correo electronico.</t>
+  </si>
+  <si>
+    <t>Necesito acceder a la aplicación web con mi cuenta de usuario y mi contraseña que ya han sido registrados en la base de datos.</t>
+  </si>
+  <si>
+    <t>Con la finalidad mantener la seguridad de mi información personal y de mis mascotas.</t>
+  </si>
+  <si>
+    <t>Con la finalidad de mostrar la información de forma ordena y agradable al usuario.</t>
+  </si>
+  <si>
+    <t>Con la finalidad de mantener mi información personal y de mis mascotas almacenadas en la cuenta de usuario.</t>
+  </si>
+  <si>
+    <t>Con la finalidad de realizar el modelo de negocio de la aplicación es necesario la busqueda de candidatos para el cruce entre mascotas.</t>
+  </si>
+  <si>
+    <t>Con la finalidad de dar soporte técnico o ayuda al usuario.</t>
+  </si>
+  <si>
+    <t>Con la finalizadad de mejorar los tiempos de busquedas de las mascotas de los usuarios.</t>
+  </si>
+  <si>
+    <t>Con la finalidad de penalizar el mal comportamiento del usuario y uso indebido de la aplicación web.</t>
+  </si>
+  <si>
+    <t>Con la finalidad de brindar mas información del dueño de la mascota candidata para acordar el cruce entre las mascotas.</t>
+  </si>
+  <si>
+    <t>Necesito ver la reputación que pueda tener el dueño u opiniones de otros usuarios con respecto al trato de esta persona; así, si el estado de su mascota se encuentra sano, limpio y bien alimentado.</t>
+  </si>
+  <si>
+    <t>Necesito ver información mas detalla de las mascotas que quiero escoger para el cruce como: ¿A quien le pertenece la mascota?, ¿Cómo me contacto con el dueño?, ¿Por qué distrito vive el dueño?, tambien un album de fotos de la mascota para saber en que condiciones se encuentra.</t>
+  </si>
+  <si>
+    <t>Necesito permitir mostrar un panel de control con un menu de opciones; y pueda ver mi perfil de usuario, mis mascotas y configuraciones.</t>
+  </si>
+  <si>
+    <t>Necesito realizar busquedas de canes según los filtros que establezca para la busqueda que pueden ser: raza, sexo, edad, peso y  ubicación del dueño.</t>
+  </si>
+  <si>
+    <t>Necesito saber el motivo por el cual no puedo acceder a su cuenta de usuario debido a inactividad, mal comportamiento u otros casos; además, me permita proceder a una solución si hubiera oportunidad.</t>
+  </si>
+  <si>
+    <t>Necesito eliminar cuentas de usuarios inactivos que no cuenta con una membresia de pago.</t>
+  </si>
+  <si>
+    <t>Necesito bloquear usuarios que presenten un comportamiento indebido para evitar la mala experiencia de los usuarios en el sitio. Dentro de la web se considera mal comportamiento. Por ejemplo, escribir una publicación ofendiendo a la mascota o al dueño. Proporcionar información falsa en alguna publicación realizada. Denunciar de forma errónea y/o sin responsabilidad algúna al usuario sin que este allá cometido algún mal comportamiento.</t>
+  </si>
+  <si>
+    <t>Con la finalidad de asegurar al usuario si debe proceder a un acuerdo con el dueño de la mascota candidata.</t>
   </si>
 </sst>
 </file>
@@ -164,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,7 +220,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -464,98 +506,158 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C11"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="80" customWidth="1"/>
-    <col min="4" max="4" width="54.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="5" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>19</v>
+    <row r="2" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="195" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="90" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>8</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando historias de usuario para el 2do sprint
</commit_message>
<xml_diff>
--- a/Documentos/PETAPP_HU_01.xlsx
+++ b/Documentos/PETAPP_HU_01.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elvis\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="12420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19170" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Historias de usuario" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>HU01</t>
   </si>
@@ -107,28 +102,40 @@
     <t>Necesito ver información mas detalla de las mascotas que quiero escoger para el cruce como: ¿A quien le pertenece la mascota?, ¿Cómo me contacto con el dueño?, ¿Por qué distrito vive el dueño?, tambien un album de fotos de la mascota para saber en que condiciones se encuentra.</t>
   </si>
   <si>
-    <t>Necesito permitir mostrar un panel de control con un menu de opciones; y pueda ver mi perfil de usuario, mis mascotas y configuraciones.</t>
-  </si>
-  <si>
     <t>Necesito realizar busquedas de canes según los filtros que establezca para la busqueda que pueden ser: raza, sexo, edad, peso y  ubicación del dueño.</t>
   </si>
   <si>
-    <t>Necesito saber el motivo por el cual no puedo acceder a su cuenta de usuario debido a inactividad, mal comportamiento u otros casos; además, me permita proceder a una solución si hubiera oportunidad.</t>
-  </si>
-  <si>
-    <t>Necesito eliminar cuentas de usuarios inactivos que no cuenta con una membresia de pago.</t>
-  </si>
-  <si>
     <t>Necesito bloquear usuarios que presenten un comportamiento indebido para evitar la mala experiencia de los usuarios en el sitio. Dentro de la web se considera mal comportamiento. Por ejemplo, escribir una publicación ofendiendo a la mascota o al dueño. Proporcionar información falsa en alguna publicación realizada. Denunciar de forma errónea y/o sin responsabilidad algúna al usuario sin que este allá cometido algún mal comportamiento.</t>
   </si>
   <si>
     <t>Con la finalidad de asegurar al usuario si debe proceder a un acuerdo con el dueño de la mascota candidata.</t>
+  </si>
+  <si>
+    <t>Necesito saber el motivo por el cual no puedo acceder a mi cuenta de usuario debido a inactividad, mal comportamiento u otros casos; además, me permita proceder a una solución si hubiera oportunidad.</t>
+  </si>
+  <si>
+    <t>Necesito eliminar cuentas de usuarios inactivos que no cuentan con una membresia de pago.</t>
+  </si>
+  <si>
+    <t>Necesito ver un panel de control con un menu de opciones; y pueda ver mi perfil de usuario, mis mascotas y configuraciones.</t>
+  </si>
+  <si>
+    <t>Como un usuario o administrador</t>
+  </si>
+  <si>
+    <t>Necesito poder cerrar la sesion de mi cuenta logeada</t>
+  </si>
+  <si>
+    <t>Con la finalidad de finalizar mis operaciónes y asegurar el cierre de mi sesion en la web.</t>
+  </si>
+  <si>
+    <t>HU10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -286,7 +293,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -321,7 +328,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -498,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,10 +513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,7 +577,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>18</v>
@@ -584,7 +591,7 @@
         <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>20</v>
@@ -598,7 +605,7 @@
         <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>21</v>
@@ -612,7 +619,7 @@
         <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>22</v>
@@ -626,7 +633,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>23</v>
@@ -657,7 +664,21 @@
         <v>25</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agregando sprint backlogs 1 y 2
</commit_message>
<xml_diff>
--- a/Documentos/PETAPP_HU_01.xlsx
+++ b/Documentos/PETAPP_HU_01.xlsx
@@ -123,13 +123,13 @@
     <t>Como un usuario o administrador</t>
   </si>
   <si>
-    <t>Necesito poder cerrar la sesion de mi cuenta logeada</t>
-  </si>
-  <si>
     <t>Con la finalidad de finalizar mis operaciónes y asegurar el cierre de mi sesion en la web.</t>
   </si>
   <si>
     <t>HU10</t>
+  </si>
+  <si>
+    <t>Necesito poder cerrar la sesion de mi cuenta logeada y retornar a la web principal</t>
   </si>
 </sst>
 </file>
@@ -505,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,16 +669,16 @@
     </row>
     <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>33</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>